<commit_message>
Boss battle camera change
</commit_message>
<xml_diff>
--- a/Data/Monster.xlsx
+++ b/Data/Monster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BroGame\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67780AD9-AE77-4B3F-9A5D-71CCCD96B2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0083C0A0-5DBE-4EAC-A61C-A23BD970979E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85F11096-AC3F-4D9D-B598-BE09DDB71694}"/>
+    <workbookView xWindow="8490" yWindow="4095" windowWidth="21600" windowHeight="11385" xr2:uid="{85F11096-AC3F-4D9D-B598-BE09DDB71694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,10 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Rapter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BlueFly</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Game/Character/Monster/Rapter/BRapter_BP.BRapter_BP_C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/Game/Character/Monster/BlueFly/BBlueFly_BP.BBlueFly_BP_C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -130,6 +122,30 @@
   </si>
   <si>
     <t>/Game/Character/Monster/WhiteMinion/BWhiteMinion_BP.BWhiteMinion_BP_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuperWhiteMinion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuperBlackMinion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Character/Monster/SuperWhiteMinion/BSuperWhiteMinion_BP.BSuperWhiteMinion_BP_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Character/Monster/SuperBlackMinion/BSuperBlackMinion_BP.BSuperBlackMinion_BP_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raptor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Character/Monster/Rapter/BRapter_BP.BRaptor_BP_C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,7 +529,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -533,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -545,16 +561,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -562,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3">
         <v>60</v>
@@ -591,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>80</v>
@@ -620,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>80</v>
@@ -649,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3">
         <v>100</v>
@@ -678,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3">
         <v>60</v>
@@ -704,10 +720,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3">
         <v>120</v>
@@ -733,10 +749,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3">
         <v>30</v>
@@ -762,10 +778,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>80</v>
@@ -790,22 +806,62 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-100</v>
+      </c>
+      <c r="F10" s="2">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2">
+        <v>100</v>
+      </c>
+      <c r="H10" s="2">
+        <v>200</v>
+      </c>
+      <c r="I10" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3">
+        <v>100</v>
+      </c>
+      <c r="D11" s="3">
+        <v>70</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-100</v>
+      </c>
+      <c r="F11" s="2">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2">
+        <v>200</v>
+      </c>
+      <c r="H11" s="2">
+        <v>200</v>
+      </c>
+      <c r="I11" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>

</xml_diff>